<commit_message>
Agrupamiento de datos por semana
</commit_message>
<xml_diff>
--- a/Data/Output/datos.xlsx
+++ b/Data/Output/datos.xlsx
@@ -486,10 +486,8 @@
           <t>941</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11012024 </t>
-        </is>
+      <c r="B2" t="n">
+        <v>11012024</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -503,11 +501,7 @@
           <t>35,783.00</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
           <t>5293</t>
@@ -525,10 +519,8 @@
           <t>EDD</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11012024 </t>
-        </is>
+      <c r="B3" t="n">
+        <v>11012024</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -537,11 +529,7 @@
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
           <t>4,438.24</t>
@@ -560,10 +548,8 @@
           <t>general</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>11012024</t>
-        </is>
+      <c r="B4" t="n">
+        <v>11012024</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -591,10 +577,8 @@
           <t>941</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11082024 </t>
-        </is>
+      <c r="B5" t="n">
+        <v>11082024</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -608,11 +592,7 @@
           <t>36,233.65</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
           <t>5293</t>
@@ -630,10 +610,8 @@
           <t>EDD</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11082024 </t>
-        </is>
+      <c r="B6" t="n">
+        <v>11082024</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -642,11 +620,7 @@
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
           <t>4,416.39</t>
@@ -665,10 +639,8 @@
           <t>general</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>11082024</t>
-        </is>
+      <c r="B7" t="n">
+        <v>11082024</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -696,10 +668,8 @@
           <t>941</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11152024  </t>
-        </is>
+      <c r="B8" t="n">
+        <v>11152024</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -713,11 +683,7 @@
           <t>38,771.93</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
           <t>5293</t>
@@ -735,10 +701,8 @@
           <t>EDD</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11152024 </t>
-        </is>
+      <c r="B9" t="n">
+        <v>11152024</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -747,11 +711,7 @@
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
           <t>4,793.73</t>
@@ -770,10 +730,8 @@
           <t>general</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>11152024</t>
-        </is>
+      <c r="B10" t="n">
+        <v>11152024</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -801,10 +759,8 @@
           <t>941</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11222024 </t>
-        </is>
+      <c r="B11" t="n">
+        <v>11222024</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -818,11 +774,7 @@
           <t>37,915.74</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
           <t>5293</t>
@@ -840,10 +792,8 @@
           <t>EDD</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11222024 </t>
-        </is>
+      <c r="B12" t="n">
+        <v>11222024</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -852,11 +802,7 @@
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
           <t>4,702.90</t>
@@ -875,10 +821,8 @@
           <t>general</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>11222024</t>
-        </is>
+      <c r="B13" t="n">
+        <v>11222024</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -906,10 +850,8 @@
           <t>941</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11292024 </t>
-        </is>
+      <c r="B14" t="n">
+        <v>11292024</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -923,11 +865,7 @@
           <t>41,179.84</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
           <t>5293</t>
@@ -945,10 +883,8 @@
           <t>EDD</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11292024 </t>
-        </is>
+      <c r="B15" t="n">
+        <v>11292024</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -957,11 +893,7 @@
       </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
           <t>5,151.26</t>
@@ -980,10 +912,8 @@
           <t>general</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>11292024</t>
-        </is>
+      <c r="B16" t="n">
+        <v>11292024</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Arreglar Archivos-Cliente de salida
</commit_message>
<xml_diff>
--- a/Data/Output/datos.xlsx
+++ b/Data/Output/datos.xlsx
@@ -491,25 +491,25 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ALEJANDRA S FASHIÓON INC</t>
+          <t>AVINA PRODUCE TIN: xxxxx8949</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>35,783.00</t>
+          <t>546.52</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>5293</t>
+          <t>7888</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2024-11-08</t>
+          <t>2024-11-06</t>
         </is>
       </c>
     </row>
@@ -524,7 +524,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ALEJANDRA'S FASHIOÓN, INC.</t>
+          <t>AVINA PRODUCE INC</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
@@ -532,13 +532,13 @@
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>4,438.24</t>
+          <t>72.92</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2024-11-08</t>
+          <t>2024-11-06</t>
         </is>
       </c>
     </row>
@@ -553,17 +553,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ALEJANDRAS FASHION INC</t>
+          <t>AVINA PRODUCE, INC.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>35783.00</t>
+          <t>546.52</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>4438.24</t>
+          <t>72.92</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -582,20 +582,20 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ALEJANDRA S FASHIÓON INC</t>
+          <t>AVINA PRODUCE TIN: xxxxx8949</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>36,233.65</t>
+          <t>546.52</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
-          <t>5293</t>
+          <t>7888</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -615,7 +615,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ALEJANDRA'S FASHIOÓN, INC.</t>
+          <t>AVINA PRODUCE INC</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -623,7 +623,7 @@
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>4,416.39</t>
+          <t>72.92</t>
         </is>
       </c>
       <c r="H6" t="inlineStr"/>
@@ -644,17 +644,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ALEJANDRAS FASHION INC</t>
+          <t>AVINA PRODUCE, INC.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>36233.65</t>
+          <t>546.52</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>4416.39</t>
+          <t>72.92</t>
         </is>
       </c>
       <c r="F7" t="inlineStr"/>
@@ -673,20 +673,20 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ALEJANDRA S FASHIÓON INC</t>
+          <t>AVINA PRODUCE TIN: xxxxx8949</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>38,771.93</t>
+          <t>546.52</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
-          <t>5293</t>
+          <t>7888</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -706,7 +706,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ALEJANDRA'S FASHIOÓN, INC.</t>
+          <t>AVINA PRODUCE INC</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -714,7 +714,7 @@
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
-          <t>4,793.73</t>
+          <t>72.92</t>
         </is>
       </c>
       <c r="H9" t="inlineStr"/>
@@ -735,17 +735,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ALEJANDRAS FASHION INC</t>
+          <t>AVINA PRODUCE, INC.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>38771.93</t>
+          <t>546.52</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>4793.73</t>
+          <t>72.92</t>
         </is>
       </c>
       <c r="F10" t="inlineStr"/>
@@ -764,20 +764,20 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ALEJANDRA S FASHIÓON INC</t>
+          <t>AVINA PRODUCE TIN: xxxxx8949</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>37,915.74</t>
+          <t>546.52</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t>5293</t>
+          <t>7888</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -797,7 +797,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ALEJANDRA'S FASHIOÓN, INC.</t>
+          <t>AVINA PRODUCE INC</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -805,7 +805,7 @@
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>4,702.90</t>
+          <t>72.92</t>
         </is>
       </c>
       <c r="H12" t="inlineStr"/>
@@ -826,17 +826,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ALEJANDRAS FASHION INC</t>
+          <t>AVINA PRODUCE, INC.</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>37915.74</t>
+          <t>546.52</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>4702.90</t>
+          <t>72.92</t>
         </is>
       </c>
       <c r="F13" t="inlineStr"/>
@@ -855,20 +855,20 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ALEJANDRA S FASHIÓON INC</t>
+          <t>AVINA PRODUCE</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>41,179.84</t>
+          <t>1,426.00</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
-          <t>5293</t>
+          <t>7888</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -888,7 +888,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ALEJANDRA'S FASHIOÓN, INC.</t>
+          <t>AVINA PRODUCE INC</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -896,7 +896,7 @@
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>5,151.26</t>
+          <t>72.92</t>
         </is>
       </c>
       <c r="H15" t="inlineStr"/>
@@ -917,17 +917,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ALEJANDRAS FASHION INC</t>
+          <t>AVINA PRODUCE, INC.</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>41179.84</t>
+          <t>546.52</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>5151.17</t>
+          <t>72.92</t>
         </is>
       </c>
       <c r="F16" t="inlineStr"/>

</xml_diff>